<commit_message>
mod(pdac excel sheet): updated the PDAC panel sheet with a description
</commit_message>
<xml_diff>
--- a/data/PDAC/PDAC_panel.xlsx
+++ b/data/PDAC/PDAC_panel.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aero_user/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/psashittal/research/constrained-Dollo/data/PDAC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B15D0DC-D6FB-D24B-9265-2BD3FAFED1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BAF344-AE93-E84F-A257-E02360865FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Design-3359_exon_coverage" sheetId="1" r:id="rId1"/>
+    <sheet name="Description_of_table" sheetId="2" r:id="rId1"/>
+    <sheet name="Design-3359_exon_coverage" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Design-3359_exon_coverage'!$A$1:$G$658</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Design-3359_exon_coverage'!$A$1:$G$658</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1978" uniqueCount="894">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="896">
   <si>
     <t>chr1</t>
   </si>
@@ -2705,13 +2706,22 @@
   </si>
   <si>
     <t>gene_name</t>
+  </si>
+  <si>
+    <t>Description:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In order to query how well our targeted panel covers the exonic regions of our genes of interest, we ran `bedtools intersect` on the panel insert file against all hg19 canonical exons downloaded from UCSC Table Browser, which simply found the intersection of the two’s genomic regions. The panel insert file’s original columns are the first four columns of PDAC_panel.xlsx, while the UCSC hg19 canonical exons file’s original columns are the last three columns. 
+Two caveats are: 
+(1) for the hg19 canonical exons from UCSC, each unique genomic region (e.g. chr17:7579309-7579339) could map to different genes and exons (e.g. HV941444 and TP53).
+(2) some amplicons, AMPL115428 being an example, do not intersect with any hg19 canonical exon. Hence bedtools will output “-1” and “.” to last three columns. These amplicons, however, either map to non-canonical exons which would still transcribe as alternate mRNA transcripts, or map to non-exonic region of genes of interest which would still add confidence to calling copy number variation (CNV) of the gene as a whole. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2842,6 +2852,12 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3224,10 +3240,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3582,10 +3607,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56DC72EF-C5EF-0941-80AA-1FB2B7FB0C7A}">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:M2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>894</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" ht="168" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>895</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:M2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G658"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>